<commit_message>
Dang Hieu - Bản vá
</commit_message>
<xml_diff>
--- a/Bieu_do_Gantt (2).xlsx
+++ b/Bieu_do_Gantt (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hoc\cnpm\NV1\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27A10E6B-F46A-4A55-9463-11ED40D24695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B566A2-413F-4ED8-9E93-AC8587893D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD79B028-C1D6-4A85-92DF-F76FA84083C8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>STT</t>
   </si>
@@ -42,28 +42,7 @@
     <t>Công việc</t>
   </si>
   <si>
-    <t>Lập kế hoạch</t>
-  </si>
-  <si>
-    <t>Danh sách yêu cầu phần mềm</t>
-  </si>
-  <si>
-    <t>Đặc tả yêu cầu</t>
-  </si>
-  <si>
-    <t>Phân tích thiết kế</t>
-  </si>
-  <si>
-    <t>Lập trình</t>
-  </si>
-  <si>
-    <t>Kiểm thử</t>
-  </si>
-  <si>
     <t>Ngày bắt đầu</t>
-  </si>
-  <si>
-    <t>Thời gian dự kiến(ngày)</t>
   </si>
   <si>
     <t>Ngày kết thúc</t>
@@ -72,7 +51,32 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Ngày bắt đầu công việc</t>
+    <t>Danh sách yêu 
+cầu phần mềm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lập kế hoạch
+</t>
+  </si>
+  <si>
+    <t>Đặc tả yêu
+cầu</t>
+  </si>
+  <si>
+    <t>Phân tích thiết
+kế</t>
+  </si>
+  <si>
+    <t>Phân tích thiết 
+kế</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lập trình
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm thử
+</t>
   </si>
 </sst>
 </file>
@@ -80,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="d"/>
-    <numFmt numFmtId="167" formatCode="ddd\,\ d\-mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ d\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -136,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,11 +185,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,13 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -214,7 +230,7 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,6 +238,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,33 +562,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75546C92-5683-469D-B7F8-4742F2A4F5A8}">
-  <dimension ref="A3:DF158"/>
+  <dimension ref="A3:DE158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AW8" sqref="AW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.5546875" style="2" customWidth="1"/>
-    <col min="7" max="48" width="3" style="2" customWidth="1"/>
-    <col min="49" max="76" width="4" style="2" customWidth="1"/>
-    <col min="77" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" style="2" customWidth="1"/>
+    <col min="6" max="47" width="3" style="2" customWidth="1"/>
+    <col min="48" max="75" width="4" style="2" customWidth="1"/>
+    <col min="76" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10">
-        <v>45177</v>
-      </c>
+    <row r="3" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -670,103 +690,102 @@
       <c r="DC3" s="1"/>
       <c r="DD3" s="1"/>
       <c r="DE3" s="1"/>
-      <c r="DF3" s="1"/>
     </row>
-    <row r="4" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4">
-        <f>G5</f>
-        <v>45177</v>
+      <c r="F4" s="12">
+        <f>F5</f>
+        <v>0</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4">
-        <f t="shared" ref="N4" si="0">N5</f>
-        <v>45184</v>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12">
+        <f t="shared" ref="M4" si="0">M5</f>
+        <v>7</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4">
-        <f t="shared" ref="U4" si="1">U5</f>
-        <v>45191</v>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12">
+        <f t="shared" ref="T4" si="1">T5</f>
+        <v>14</v>
       </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4">
-        <f t="shared" ref="AB4" si="2">AB5</f>
-        <v>45198</v>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12">
+        <f t="shared" ref="AA4" si="2">AA5</f>
+        <v>21</v>
       </c>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4">
-        <f t="shared" ref="AI4" si="3">AI5</f>
-        <v>45205</v>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12">
+        <f t="shared" ref="AH4" si="3">AH5</f>
+        <v>28</v>
       </c>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4">
-        <f>AP5</f>
-        <v>45212</v>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12">
+        <f>AO5</f>
+        <v>35</v>
       </c>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
-      <c r="BA4" s="4"/>
-      <c r="BB4" s="4"/>
-      <c r="BC4" s="4"/>
-      <c r="BD4" s="4"/>
-      <c r="BE4" s="4"/>
-      <c r="BF4" s="4"/>
-      <c r="BG4" s="4"/>
-      <c r="BH4" s="4"/>
-      <c r="BI4" s="4"/>
-      <c r="BJ4" s="4"/>
-      <c r="BK4" s="4"/>
-      <c r="BL4" s="4"/>
-      <c r="BM4" s="4"/>
-      <c r="BN4" s="4"/>
-      <c r="BO4" s="4"/>
-      <c r="BP4" s="4"/>
-      <c r="BQ4" s="4"/>
-      <c r="BR4" s="4"/>
-      <c r="BS4" s="4"/>
-      <c r="BT4" s="4"/>
-      <c r="BU4" s="4"/>
-      <c r="BV4" s="4"/>
-      <c r="BW4" s="4"/>
-      <c r="BX4" s="4"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
+      <c r="AY4" s="12"/>
+      <c r="AZ4" s="12"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BC4" s="12"/>
+      <c r="BD4" s="12"/>
+      <c r="BE4" s="12"/>
+      <c r="BF4" s="12"/>
+      <c r="BG4" s="12"/>
+      <c r="BH4" s="12"/>
+      <c r="BI4" s="12"/>
+      <c r="BJ4" s="12"/>
+      <c r="BK4" s="12"/>
+      <c r="BL4" s="12"/>
+      <c r="BM4" s="12"/>
+      <c r="BN4" s="12"/>
+      <c r="BO4" s="12"/>
+      <c r="BP4" s="12"/>
+      <c r="BQ4" s="12"/>
+      <c r="BR4" s="12"/>
+      <c r="BS4" s="12"/>
+      <c r="BT4" s="12"/>
+      <c r="BU4" s="12"/>
+      <c r="BV4" s="12"/>
+      <c r="BW4" s="12"/>
+      <c r="BX4" s="1"/>
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
       <c r="CA4" s="1"/>
@@ -800,183 +819,182 @@
       <c r="DC4" s="1"/>
       <c r="DD4" s="1"/>
       <c r="DE4" s="1"/>
-      <c r="DF4" s="1"/>
     </row>
-    <row r="5" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="5">
+      <c r="F5" s="4">
         <f>$C$3</f>
-        <v>45177</v>
+        <v>0</v>
       </c>
-      <c r="H5" s="5">
-        <f>G5 + 1</f>
-        <v>45178</v>
+      <c r="G5" s="4">
+        <f>F5 + 1</f>
+        <v>1</v>
       </c>
-      <c r="I5" s="5">
-        <f t="shared" ref="I5:AV5" si="4">H5 + 1</f>
-        <v>45179</v>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:AU5" si="4">G5 + 1</f>
+        <v>2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="I5" s="4">
         <f t="shared" si="4"/>
-        <v>45180</v>
+        <v>3</v>
       </c>
-      <c r="K5" s="5">
+      <c r="J5" s="4">
         <f t="shared" si="4"/>
-        <v>45181</v>
+        <v>4</v>
       </c>
-      <c r="L5" s="5">
+      <c r="K5" s="4">
         <f t="shared" si="4"/>
-        <v>45182</v>
+        <v>5</v>
       </c>
-      <c r="M5" s="5">
+      <c r="L5" s="4">
         <f t="shared" si="4"/>
-        <v>45183</v>
+        <v>6</v>
       </c>
-      <c r="N5" s="5">
+      <c r="M5" s="4">
         <f t="shared" si="4"/>
-        <v>45184</v>
+        <v>7</v>
       </c>
-      <c r="O5" s="5">
+      <c r="N5" s="4">
         <f t="shared" si="4"/>
-        <v>45185</v>
+        <v>8</v>
       </c>
-      <c r="P5" s="5">
+      <c r="O5" s="4">
         <f t="shared" si="4"/>
-        <v>45186</v>
+        <v>9</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="P5" s="4">
         <f t="shared" si="4"/>
-        <v>45187</v>
+        <v>10</v>
       </c>
-      <c r="R5" s="5">
+      <c r="Q5" s="4">
         <f t="shared" si="4"/>
-        <v>45188</v>
+        <v>11</v>
       </c>
-      <c r="S5" s="5">
+      <c r="R5" s="4">
         <f t="shared" si="4"/>
-        <v>45189</v>
+        <v>12</v>
       </c>
-      <c r="T5" s="5">
+      <c r="S5" s="4">
         <f t="shared" si="4"/>
-        <v>45190</v>
+        <v>13</v>
       </c>
-      <c r="U5" s="5">
+      <c r="T5" s="4">
         <f t="shared" si="4"/>
-        <v>45191</v>
+        <v>14</v>
       </c>
-      <c r="V5" s="5">
+      <c r="U5" s="4">
         <f t="shared" si="4"/>
-        <v>45192</v>
+        <v>15</v>
       </c>
-      <c r="W5" s="5">
+      <c r="V5" s="4">
         <f t="shared" si="4"/>
-        <v>45193</v>
+        <v>16</v>
       </c>
-      <c r="X5" s="5">
+      <c r="W5" s="4">
         <f t="shared" si="4"/>
-        <v>45194</v>
+        <v>17</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="X5" s="4">
         <f t="shared" si="4"/>
-        <v>45195</v>
+        <v>18</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Y5" s="4">
         <f t="shared" si="4"/>
-        <v>45196</v>
+        <v>19</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="Z5" s="4">
         <f t="shared" si="4"/>
-        <v>45197</v>
+        <v>20</v>
       </c>
-      <c r="AB5" s="5">
+      <c r="AA5" s="4">
         <f t="shared" si="4"/>
-        <v>45198</v>
+        <v>21</v>
       </c>
-      <c r="AC5" s="5">
+      <c r="AB5" s="4">
         <f t="shared" si="4"/>
-        <v>45199</v>
+        <v>22</v>
       </c>
-      <c r="AD5" s="5">
+      <c r="AC5" s="4">
         <f t="shared" si="4"/>
-        <v>45200</v>
+        <v>23</v>
       </c>
-      <c r="AE5" s="5">
+      <c r="AD5" s="4">
         <f t="shared" si="4"/>
-        <v>45201</v>
+        <v>24</v>
       </c>
-      <c r="AF5" s="5">
+      <c r="AE5" s="4">
         <f t="shared" si="4"/>
-        <v>45202</v>
+        <v>25</v>
       </c>
-      <c r="AG5" s="5">
+      <c r="AF5" s="4">
         <f t="shared" si="4"/>
-        <v>45203</v>
+        <v>26</v>
       </c>
-      <c r="AH5" s="5">
+      <c r="AG5" s="4">
         <f t="shared" si="4"/>
-        <v>45204</v>
+        <v>27</v>
       </c>
-      <c r="AI5" s="5">
+      <c r="AH5" s="4">
         <f t="shared" si="4"/>
-        <v>45205</v>
+        <v>28</v>
       </c>
-      <c r="AJ5" s="5">
+      <c r="AI5" s="4">
         <f t="shared" si="4"/>
-        <v>45206</v>
+        <v>29</v>
       </c>
-      <c r="AK5" s="5">
+      <c r="AJ5" s="4">
         <f t="shared" si="4"/>
-        <v>45207</v>
+        <v>30</v>
       </c>
-      <c r="AL5" s="5">
+      <c r="AK5" s="4">
         <f t="shared" si="4"/>
-        <v>45208</v>
+        <v>31</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AL5" s="4">
         <f t="shared" si="4"/>
-        <v>45209</v>
+        <v>32</v>
       </c>
-      <c r="AN5" s="5">
+      <c r="AM5" s="4">
         <f t="shared" si="4"/>
-        <v>45210</v>
+        <v>33</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AN5" s="4">
         <f t="shared" si="4"/>
-        <v>45211</v>
+        <v>34</v>
       </c>
-      <c r="AP5" s="5">
+      <c r="AO5" s="4">
         <f t="shared" si="4"/>
-        <v>45212</v>
+        <v>35</v>
       </c>
-      <c r="AQ5" s="5">
+      <c r="AP5" s="4">
         <f t="shared" si="4"/>
-        <v>45213</v>
+        <v>36</v>
       </c>
-      <c r="AR5" s="5">
+      <c r="AQ5" s="4">
         <f t="shared" si="4"/>
-        <v>45214</v>
+        <v>37</v>
       </c>
-      <c r="AS5" s="5">
+      <c r="AR5" s="4">
         <f t="shared" si="4"/>
-        <v>45215</v>
+        <v>38</v>
       </c>
-      <c r="AT5" s="5">
+      <c r="AS5" s="4">
         <f t="shared" si="4"/>
-        <v>45216</v>
+        <v>39</v>
       </c>
-      <c r="AU5" s="5">
+      <c r="AT5" s="4">
         <f t="shared" si="4"/>
-        <v>45217</v>
+        <v>40</v>
       </c>
-      <c r="AV5" s="5">
+      <c r="AU5" s="4">
         <f t="shared" si="4"/>
-        <v>45218</v>
+        <v>41</v>
       </c>
+      <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
@@ -1004,7 +1022,7 @@
       <c r="BU5" s="3"/>
       <c r="BV5" s="3"/>
       <c r="BW5" s="3"/>
-      <c r="BX5" s="3"/>
+      <c r="BX5" s="1"/>
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
       <c r="CA5" s="1"/>
@@ -1038,193 +1056,190 @@
       <c r="DC5" s="1"/>
       <c r="DD5" s="1"/>
       <c r="DE5" s="1"/>
-      <c r="DF5" s="1"/>
     </row>
-    <row r="6" spans="1:110" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:109" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="str">
+        <f>LEFT(TEXT(F5,"ddd"),1)</f>
+        <v>S</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7" t="str">
-        <f>LEFT(TEXT(G5,"ddd"),1)</f>
+      <c r="G6" s="6" t="str">
+        <f t="shared" ref="G6:M6" si="5">LEFT(TEXT(G5,"ddd"),1)</f>
+        <v>S</v>
+      </c>
+      <c r="H6" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>M</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>T</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>W</v>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>T</v>
+      </c>
+      <c r="L6" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" ref="H6:N6" si="5">LEFT(TEXT(H5,"ddd"),1)</f>
-        <v>S</v>
-      </c>
-      <c r="I6" s="7" t="str">
+      <c r="M6" s="6" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="J6" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="N6" s="6" t="str">
+        <f t="shared" ref="N6" si="6">LEFT(TEXT(N5,"ddd"),1)</f>
+        <v>S</v>
+      </c>
+      <c r="O6" s="6" t="str">
+        <f t="shared" ref="O6" si="7">LEFT(TEXT(O5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="K6" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="P6" s="6" t="str">
+        <f t="shared" ref="P6" si="8">LEFT(TEXT(P5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="L6" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="Q6" s="6" t="str">
+        <f t="shared" ref="Q6" si="9">LEFT(TEXT(Q5,"ddd"),1)</f>
         <v>W</v>
       </c>
-      <c r="M6" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="R6" s="6" t="str">
+        <f t="shared" ref="R6" si="10">LEFT(TEXT(R5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="N6" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="S6" s="6" t="str">
+        <f t="shared" ref="S6:T6" si="11">LEFT(TEXT(S5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="O6" s="7" t="str">
-        <f t="shared" ref="O6" si="6">LEFT(TEXT(O5,"ddd"),1)</f>
+      <c r="T6" s="6" t="str">
+        <f t="shared" si="11"/>
         <v>S</v>
       </c>
-      <c r="P6" s="7" t="str">
-        <f t="shared" ref="P6" si="7">LEFT(TEXT(P5,"ddd"),1)</f>
+      <c r="U6" s="6" t="str">
+        <f t="shared" ref="U6" si="12">LEFT(TEXT(U5,"ddd"),1)</f>
         <v>S</v>
       </c>
-      <c r="Q6" s="7" t="str">
-        <f t="shared" ref="Q6" si="8">LEFT(TEXT(Q5,"ddd"),1)</f>
+      <c r="V6" s="6" t="str">
+        <f t="shared" ref="V6" si="13">LEFT(TEXT(V5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="R6" s="7" t="str">
-        <f t="shared" ref="R6" si="9">LEFT(TEXT(R5,"ddd"),1)</f>
+      <c r="W6" s="6" t="str">
+        <f t="shared" ref="W6" si="14">LEFT(TEXT(W5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="S6" s="7" t="str">
-        <f t="shared" ref="S6" si="10">LEFT(TEXT(S5,"ddd"),1)</f>
+      <c r="X6" s="6" t="str">
+        <f t="shared" ref="X6" si="15">LEFT(TEXT(X5,"ddd"),1)</f>
         <v>W</v>
       </c>
-      <c r="T6" s="7" t="str">
-        <f t="shared" ref="T6:U6" si="11">LEFT(TEXT(T5,"ddd"),1)</f>
+      <c r="Y6" s="6" t="str">
+        <f t="shared" ref="Y6" si="16">LEFT(TEXT(Y5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="U6" s="7" t="str">
-        <f t="shared" si="11"/>
+      <c r="Z6" s="6" t="str">
+        <f t="shared" ref="Z6:AA6" si="17">LEFT(TEXT(Z5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="V6" s="7" t="str">
-        <f t="shared" ref="V6" si="12">LEFT(TEXT(V5,"ddd"),1)</f>
+      <c r="AA6" s="6" t="str">
+        <f t="shared" si="17"/>
         <v>S</v>
       </c>
-      <c r="W6" s="7" t="str">
-        <f t="shared" ref="W6" si="13">LEFT(TEXT(W5,"ddd"),1)</f>
+      <c r="AB6" s="6" t="str">
+        <f t="shared" ref="AB6" si="18">LEFT(TEXT(AB5,"ddd"),1)</f>
         <v>S</v>
       </c>
-      <c r="X6" s="7" t="str">
-        <f t="shared" ref="X6" si="14">LEFT(TEXT(X5,"ddd"),1)</f>
+      <c r="AC6" s="6" t="str">
+        <f t="shared" ref="AC6" si="19">LEFT(TEXT(AC5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="Y6" s="7" t="str">
-        <f t="shared" ref="Y6" si="15">LEFT(TEXT(Y5,"ddd"),1)</f>
+      <c r="AD6" s="6" t="str">
+        <f t="shared" ref="AD6" si="20">LEFT(TEXT(AD5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="Z6" s="7" t="str">
-        <f t="shared" ref="Z6" si="16">LEFT(TEXT(Z5,"ddd"),1)</f>
+      <c r="AE6" s="6" t="str">
+        <f t="shared" ref="AE6" si="21">LEFT(TEXT(AE5,"ddd"),1)</f>
         <v>W</v>
       </c>
-      <c r="AA6" s="7" t="str">
-        <f t="shared" ref="AA6:AB6" si="17">LEFT(TEXT(AA5,"ddd"),1)</f>
+      <c r="AF6" s="6" t="str">
+        <f t="shared" ref="AF6" si="22">LEFT(TEXT(AF5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AB6" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="AG6" s="6" t="str">
+        <f t="shared" ref="AG6:AH6" si="23">LEFT(TEXT(AG5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="AC6" s="7" t="str">
-        <f t="shared" ref="AC6" si="18">LEFT(TEXT(AC5,"ddd"),1)</f>
+      <c r="AH6" s="6" t="str">
+        <f t="shared" si="23"/>
         <v>S</v>
       </c>
-      <c r="AD6" s="7" t="str">
-        <f t="shared" ref="AD6" si="19">LEFT(TEXT(AD5,"ddd"),1)</f>
+      <c r="AI6" s="6" t="str">
+        <f t="shared" ref="AI6" si="24">LEFT(TEXT(AI5,"ddd"),1)</f>
         <v>S</v>
       </c>
-      <c r="AE6" s="7" t="str">
-        <f t="shared" ref="AE6" si="20">LEFT(TEXT(AE5,"ddd"),1)</f>
+      <c r="AJ6" s="6" t="str">
+        <f t="shared" ref="AJ6" si="25">LEFT(TEXT(AJ5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="AF6" s="7" t="str">
-        <f t="shared" ref="AF6" si="21">LEFT(TEXT(AF5,"ddd"),1)</f>
+      <c r="AK6" s="6" t="str">
+        <f t="shared" ref="AK6" si="26">LEFT(TEXT(AK5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AG6" s="7" t="str">
-        <f t="shared" ref="AG6" si="22">LEFT(TEXT(AG5,"ddd"),1)</f>
+      <c r="AL6" s="6" t="str">
+        <f t="shared" ref="AL6" si="27">LEFT(TEXT(AL5,"ddd"),1)</f>
         <v>W</v>
       </c>
-      <c r="AH6" s="7" t="str">
-        <f t="shared" ref="AH6:AI6" si="23">LEFT(TEXT(AH5,"ddd"),1)</f>
+      <c r="AM6" s="6" t="str">
+        <f t="shared" ref="AM6" si="28">LEFT(TEXT(AM5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AI6" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="AN6" s="6" t="str">
+        <f t="shared" ref="AN6" si="29">LEFT(TEXT(AN5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="AJ6" s="7" t="str">
-        <f t="shared" ref="AJ6" si="24">LEFT(TEXT(AJ5,"ddd"),1)</f>
+      <c r="AO6" s="6" t="str">
+        <f>LEFT(TEXT(AO5,"ddd"),1)</f>
         <v>S</v>
       </c>
-      <c r="AK6" s="7" t="str">
-        <f t="shared" ref="AK6" si="25">LEFT(TEXT(AK5,"ddd"),1)</f>
+      <c r="AP6" s="6" t="str">
+        <f t="shared" ref="AP6" si="30">LEFT(TEXT(AP5,"ddd"),1)</f>
         <v>S</v>
       </c>
-      <c r="AL6" s="7" t="str">
-        <f t="shared" ref="AL6" si="26">LEFT(TEXT(AL5,"ddd"),1)</f>
+      <c r="AQ6" s="6" t="str">
+        <f t="shared" ref="AQ6" si="31">LEFT(TEXT(AQ5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="AM6" s="7" t="str">
-        <f t="shared" ref="AM6" si="27">LEFT(TEXT(AM5,"ddd"),1)</f>
+      <c r="AR6" s="6" t="str">
+        <f t="shared" ref="AR6" si="32">LEFT(TEXT(AR5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AN6" s="7" t="str">
-        <f t="shared" ref="AN6" si="28">LEFT(TEXT(AN5,"ddd"),1)</f>
+      <c r="AS6" s="6" t="str">
+        <f t="shared" ref="AS6" si="33">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>W</v>
       </c>
-      <c r="AO6" s="7" t="str">
-        <f t="shared" ref="AO6" si="29">LEFT(TEXT(AO5,"ddd"),1)</f>
+      <c r="AT6" s="6" t="str">
+        <f t="shared" ref="AT6" si="34">LEFT(TEXT(AT5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AP6" s="7" t="str">
-        <f>LEFT(TEXT(AP5,"ddd"),1)</f>
+      <c r="AU6" s="6" t="str">
+        <f t="shared" ref="AU6" si="35">LEFT(TEXT(AU5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="AQ6" s="7" t="str">
-        <f t="shared" ref="AQ6" si="30">LEFT(TEXT(AQ5,"ddd"),1)</f>
-        <v>S</v>
-      </c>
-      <c r="AR6" s="7" t="str">
-        <f t="shared" ref="AR6" si="31">LEFT(TEXT(AR5,"ddd"),1)</f>
-        <v>S</v>
-      </c>
-      <c r="AS6" s="7" t="str">
-        <f t="shared" ref="AS6" si="32">LEFT(TEXT(AS5,"ddd"),1)</f>
-        <v>M</v>
-      </c>
-      <c r="AT6" s="7" t="str">
-        <f t="shared" ref="AT6" si="33">LEFT(TEXT(AT5,"ddd"),1)</f>
-        <v>T</v>
-      </c>
-      <c r="AU6" s="7" t="str">
-        <f t="shared" ref="AU6" si="34">LEFT(TEXT(AU5,"ddd"),1)</f>
-        <v>W</v>
-      </c>
-      <c r="AV6" s="7" t="str">
-        <f t="shared" ref="AV6" si="35">LEFT(TEXT(AV5,"ddd"),1)</f>
-        <v>T</v>
-      </c>
+      <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
@@ -1286,69 +1301,66 @@
       <c r="DC6" s="1"/>
       <c r="DD6" s="1"/>
       <c r="DE6" s="1"/>
-      <c r="DF6" s="1"/>
     </row>
-    <row r="7" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+    <row r="7" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>2</v>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>45177</v>
       </c>
       <c r="D7" s="8">
+        <v>45184</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="11">
         <v>7</v>
       </c>
-      <c r="E7" s="9">
-        <v>45184</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="12">
-        <v>7</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="8"/>
-      <c r="AI7" s="8"/>
-      <c r="AJ7" s="8"/>
-      <c r="AK7" s="8"/>
-      <c r="AL7" s="8"/>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="8"/>
-      <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="8"/>
-      <c r="AR7" s="8"/>
-      <c r="AS7" s="8"/>
-      <c r="AT7" s="8"/>
-      <c r="AU7" s="8"/>
-      <c r="AV7" s="8"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="7"/>
+      <c r="AT7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
@@ -1410,69 +1422,66 @@
       <c r="DC7" s="1"/>
       <c r="DD7" s="1"/>
       <c r="DE7" s="1"/>
-      <c r="DF7" s="1"/>
     </row>
-    <row r="8" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+    <row r="8" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>2</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
+      <c r="B8" s="14" t="s">
+        <v>5</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>45185</v>
       </c>
       <c r="D8" s="8">
+        <v>45188</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="11">
         <v>3</v>
       </c>
-      <c r="E8" s="9">
-        <v>45188</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="12">
-        <v>3</v>
-      </c>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-      <c r="AR8" s="8"/>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
       <c r="AY8" s="1"/>
@@ -1534,71 +1543,68 @@
       <c r="DC8" s="1"/>
       <c r="DD8" s="1"/>
       <c r="DE8" s="1"/>
-      <c r="DF8" s="1"/>
     </row>
-    <row r="9" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+    <row r="9" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>4</v>
+      <c r="B9" s="14" t="s">
+        <v>7</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>45189</v>
       </c>
       <c r="D9" s="8">
+        <v>45191</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="11">
         <v>2</v>
       </c>
-      <c r="E9" s="9">
-        <v>45191</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="12">
-        <v>2</v>
-      </c>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="8"/>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="8"/>
-      <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="8"/>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
+      <c r="AN9" s="7"/>
+      <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
       <c r="AY9" s="1"/>
@@ -1660,69 +1666,66 @@
       <c r="DC9" s="1"/>
       <c r="DD9" s="1"/>
       <c r="DE9" s="1"/>
-      <c r="DF9" s="1"/>
     </row>
-    <row r="10" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+    <row r="10" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>5</v>
+      <c r="B10" s="14" t="s">
+        <v>8</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>45192</v>
       </c>
       <c r="D10" s="8">
+        <v>45196</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="11">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
-        <v>45196</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="12">
-        <v>4</v>
-      </c>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-      <c r="AI10" s="8"/>
-      <c r="AJ10" s="8"/>
-      <c r="AK10" s="8"/>
-      <c r="AL10" s="8"/>
-      <c r="AM10" s="8"/>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="8"/>
-      <c r="AR10" s="8"/>
-      <c r="AS10" s="8"/>
-      <c r="AT10" s="8"/>
-      <c r="AU10" s="8"/>
-      <c r="AV10" s="8"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="7"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7"/>
+      <c r="AR10" s="7"/>
+      <c r="AS10" s="7"/>
+      <c r="AT10" s="7"/>
+      <c r="AU10" s="7"/>
+      <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
       <c r="AX10" s="1"/>
       <c r="AY10" s="1"/>
@@ -1784,69 +1787,66 @@
       <c r="DC10" s="1"/>
       <c r="DD10" s="1"/>
       <c r="DE10" s="1"/>
-      <c r="DF10" s="1"/>
     </row>
-    <row r="11" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+    <row r="11" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>6</v>
+      <c r="B11" s="14" t="s">
+        <v>10</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>45197</v>
       </c>
       <c r="D11" s="8">
+        <v>45199</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="11">
         <v>2</v>
       </c>
-      <c r="E11" s="9">
-        <v>45199</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="12">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="12"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
-      <c r="AH11" s="8"/>
-      <c r="AI11" s="8"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="8"/>
-      <c r="AL11" s="8"/>
-      <c r="AM11" s="8"/>
-      <c r="AN11" s="8"/>
-      <c r="AO11" s="8"/>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="8"/>
-      <c r="AR11" s="8"/>
-      <c r="AS11" s="8"/>
-      <c r="AT11" s="8"/>
-      <c r="AU11" s="8"/>
-      <c r="AV11" s="8"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="7"/>
+      <c r="AS11" s="7"/>
+      <c r="AT11" s="7"/>
+      <c r="AU11" s="7"/>
+      <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
       <c r="AX11" s="1"/>
       <c r="AY11" s="1"/>
@@ -1908,69 +1908,66 @@
       <c r="DC11" s="1"/>
       <c r="DD11" s="1"/>
       <c r="DE11" s="1"/>
-      <c r="DF11" s="1"/>
     </row>
-    <row r="12" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+    <row r="12" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
+      <c r="B12" s="14" t="s">
+        <v>11</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>45200</v>
       </c>
       <c r="D12" s="8">
+        <v>45202</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="11">
         <v>2</v>
       </c>
-      <c r="E12" s="9">
-        <v>45202</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="12">
-        <v>2</v>
-      </c>
-      <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="8"/>
-      <c r="AH12" s="8"/>
-      <c r="AI12" s="8"/>
-      <c r="AJ12" s="8"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="8"/>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="8"/>
-      <c r="AO12" s="8"/>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="8"/>
-      <c r="AR12" s="8"/>
-      <c r="AS12" s="8"/>
-      <c r="AT12" s="8"/>
-      <c r="AU12" s="8"/>
-      <c r="AV12" s="8"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7"/>
+      <c r="AL12" s="7"/>
+      <c r="AM12" s="7"/>
+      <c r="AN12" s="7"/>
+      <c r="AO12" s="7"/>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="7"/>
+      <c r="AS12" s="7"/>
+      <c r="AT12" s="7"/>
+      <c r="AU12" s="7"/>
+      <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
       <c r="AY12" s="1"/>
@@ -2032,69 +2029,66 @@
       <c r="DC12" s="1"/>
       <c r="DD12" s="1"/>
       <c r="DE12" s="1"/>
-      <c r="DF12" s="1"/>
     </row>
-    <row r="13" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+    <row r="13" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>4</v>
+      <c r="B13" s="14" t="s">
+        <v>7</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>45203</v>
       </c>
       <c r="D13" s="8">
+        <v>45205</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="11">
         <v>2</v>
       </c>
-      <c r="E13" s="9">
-        <v>45205</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="12">
-        <v>2</v>
-      </c>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="8"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="8"/>
-      <c r="AR13" s="8"/>
-      <c r="AS13" s="8"/>
-      <c r="AT13" s="8"/>
-      <c r="AU13" s="8"/>
-      <c r="AV13" s="8"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7"/>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="7"/>
+      <c r="AN13" s="7"/>
+      <c r="AO13" s="7"/>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
+      <c r="AS13" s="7"/>
+      <c r="AT13" s="7"/>
+      <c r="AU13" s="7"/>
+      <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
       <c r="AY13" s="1"/>
@@ -2156,69 +2150,66 @@
       <c r="DC13" s="1"/>
       <c r="DD13" s="1"/>
       <c r="DE13" s="1"/>
-      <c r="DF13" s="1"/>
     </row>
-    <row r="14" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+    <row r="14" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>8</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>5</v>
+      <c r="B14" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>45206</v>
       </c>
       <c r="D14" s="8">
+        <v>45210</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="11">
         <v>4</v>
       </c>
-      <c r="E14" s="9">
-        <v>45210</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="12">
-        <v>4</v>
-      </c>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
-      <c r="AN14" s="12"/>
-      <c r="AO14" s="8"/>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="8"/>
-      <c r="AR14" s="8"/>
-      <c r="AS14" s="8"/>
-      <c r="AT14" s="8"/>
-      <c r="AU14" s="8"/>
-      <c r="AV14" s="8"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="7"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
+      <c r="AS14" s="7"/>
+      <c r="AT14" s="7"/>
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
       <c r="AY14" s="1"/>
@@ -2280,69 +2271,66 @@
       <c r="DC14" s="1"/>
       <c r="DD14" s="1"/>
       <c r="DE14" s="1"/>
-      <c r="DF14" s="1"/>
     </row>
-    <row r="15" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+    <row r="15" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>6</v>
+      <c r="B15" s="14" t="s">
+        <v>10</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>45211</v>
       </c>
       <c r="D15" s="8">
+        <v>45213</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="11">
         <v>2</v>
       </c>
-      <c r="E15" s="9">
-        <v>45213</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="8"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="8"/>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="12">
-        <v>2</v>
-      </c>
-      <c r="AP15" s="12"/>
-      <c r="AQ15" s="12"/>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
-      <c r="AU15" s="8"/>
-      <c r="AV15" s="8"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="7"/>
+      <c r="AR15" s="7"/>
+      <c r="AS15" s="7"/>
+      <c r="AT15" s="7"/>
+      <c r="AU15" s="7"/>
+      <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
       <c r="AY15" s="1"/>
@@ -2404,69 +2392,66 @@
       <c r="DC15" s="1"/>
       <c r="DD15" s="1"/>
       <c r="DE15" s="1"/>
-      <c r="DF15" s="1"/>
     </row>
-    <row r="16" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+    <row r="16" spans="1:109" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
+      <c r="B16" s="14" t="s">
+        <v>11</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>45214</v>
       </c>
       <c r="D16" s="8">
+        <v>45216</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+      <c r="AO16" s="7"/>
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="11">
         <v>2</v>
       </c>
-      <c r="E16" s="9">
-        <v>45216</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="8"/>
-      <c r="AR16" s="12">
-        <v>2</v>
-      </c>
-      <c r="AS16" s="12"/>
-      <c r="AT16" s="12"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
+      <c r="AR16" s="11"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="7"/>
+      <c r="AU16" s="7"/>
+      <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
       <c r="AY16" s="1"/>
@@ -2528,9 +2513,8 @@
       <c r="DC16" s="1"/>
       <c r="DD16" s="1"/>
       <c r="DE16" s="1"/>
-      <c r="DF16" s="1"/>
     </row>
-    <row r="17" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2640,9 +2624,8 @@
       <c r="DC17" s="1"/>
       <c r="DD17" s="1"/>
       <c r="DE17" s="1"/>
-      <c r="DF17" s="1"/>
     </row>
-    <row r="18" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2752,9 +2735,8 @@
       <c r="DC18" s="1"/>
       <c r="DD18" s="1"/>
       <c r="DE18" s="1"/>
-      <c r="DF18" s="1"/>
     </row>
-    <row r="19" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2864,9 +2846,8 @@
       <c r="DC19" s="1"/>
       <c r="DD19" s="1"/>
       <c r="DE19" s="1"/>
-      <c r="DF19" s="1"/>
     </row>
-    <row r="20" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2976,9 +2957,8 @@
       <c r="DC20" s="1"/>
       <c r="DD20" s="1"/>
       <c r="DE20" s="1"/>
-      <c r="DF20" s="1"/>
     </row>
-    <row r="21" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3088,9 +3068,8 @@
       <c r="DC21" s="1"/>
       <c r="DD21" s="1"/>
       <c r="DE21" s="1"/>
-      <c r="DF21" s="1"/>
     </row>
-    <row r="22" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3200,9 +3179,8 @@
       <c r="DC22" s="1"/>
       <c r="DD22" s="1"/>
       <c r="DE22" s="1"/>
-      <c r="DF22" s="1"/>
     </row>
-    <row r="23" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3312,9 +3290,8 @@
       <c r="DC23" s="1"/>
       <c r="DD23" s="1"/>
       <c r="DE23" s="1"/>
-      <c r="DF23" s="1"/>
     </row>
-    <row r="24" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3424,9 +3401,8 @@
       <c r="DC24" s="1"/>
       <c r="DD24" s="1"/>
       <c r="DE24" s="1"/>
-      <c r="DF24" s="1"/>
     </row>
-    <row r="25" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3536,9 +3512,8 @@
       <c r="DC25" s="1"/>
       <c r="DD25" s="1"/>
       <c r="DE25" s="1"/>
-      <c r="DF25" s="1"/>
     </row>
-    <row r="26" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3648,9 +3623,8 @@
       <c r="DC26" s="1"/>
       <c r="DD26" s="1"/>
       <c r="DE26" s="1"/>
-      <c r="DF26" s="1"/>
     </row>
-    <row r="27" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3760,9 +3734,8 @@
       <c r="DC27" s="1"/>
       <c r="DD27" s="1"/>
       <c r="DE27" s="1"/>
-      <c r="DF27" s="1"/>
     </row>
-    <row r="28" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3872,9 +3845,8 @@
       <c r="DC28" s="1"/>
       <c r="DD28" s="1"/>
       <c r="DE28" s="1"/>
-      <c r="DF28" s="1"/>
     </row>
-    <row r="29" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3984,9 +3956,8 @@
       <c r="DC29" s="1"/>
       <c r="DD29" s="1"/>
       <c r="DE29" s="1"/>
-      <c r="DF29" s="1"/>
     </row>
-    <row r="30" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4096,9 +4067,8 @@
       <c r="DC30" s="1"/>
       <c r="DD30" s="1"/>
       <c r="DE30" s="1"/>
-      <c r="DF30" s="1"/>
     </row>
-    <row r="31" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4208,9 +4178,8 @@
       <c r="DC31" s="1"/>
       <c r="DD31" s="1"/>
       <c r="DE31" s="1"/>
-      <c r="DF31" s="1"/>
     </row>
-    <row r="32" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4320,9 +4289,8 @@
       <c r="DC32" s="1"/>
       <c r="DD32" s="1"/>
       <c r="DE32" s="1"/>
-      <c r="DF32" s="1"/>
     </row>
-    <row r="33" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -4432,9 +4400,8 @@
       <c r="DC33" s="1"/>
       <c r="DD33" s="1"/>
       <c r="DE33" s="1"/>
-      <c r="DF33" s="1"/>
     </row>
-    <row r="34" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -4544,9 +4511,8 @@
       <c r="DC34" s="1"/>
       <c r="DD34" s="1"/>
       <c r="DE34" s="1"/>
-      <c r="DF34" s="1"/>
     </row>
-    <row r="35" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -4656,9 +4622,8 @@
       <c r="DC35" s="1"/>
       <c r="DD35" s="1"/>
       <c r="DE35" s="1"/>
-      <c r="DF35" s="1"/>
     </row>
-    <row r="36" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -4768,9 +4733,8 @@
       <c r="DC36" s="1"/>
       <c r="DD36" s="1"/>
       <c r="DE36" s="1"/>
-      <c r="DF36" s="1"/>
     </row>
-    <row r="37" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -4880,9 +4844,8 @@
       <c r="DC37" s="1"/>
       <c r="DD37" s="1"/>
       <c r="DE37" s="1"/>
-      <c r="DF37" s="1"/>
     </row>
-    <row r="38" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4992,9 +4955,8 @@
       <c r="DC38" s="1"/>
       <c r="DD38" s="1"/>
       <c r="DE38" s="1"/>
-      <c r="DF38" s="1"/>
     </row>
-    <row r="39" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -5104,9 +5066,8 @@
       <c r="DC39" s="1"/>
       <c r="DD39" s="1"/>
       <c r="DE39" s="1"/>
-      <c r="DF39" s="1"/>
     </row>
-    <row r="40" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -5216,9 +5177,8 @@
       <c r="DC40" s="1"/>
       <c r="DD40" s="1"/>
       <c r="DE40" s="1"/>
-      <c r="DF40" s="1"/>
     </row>
-    <row r="41" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -5328,9 +5288,8 @@
       <c r="DC41" s="1"/>
       <c r="DD41" s="1"/>
       <c r="DE41" s="1"/>
-      <c r="DF41" s="1"/>
     </row>
-    <row r="42" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -5440,9 +5399,8 @@
       <c r="DC42" s="1"/>
       <c r="DD42" s="1"/>
       <c r="DE42" s="1"/>
-      <c r="DF42" s="1"/>
     </row>
-    <row r="43" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5552,9 +5510,8 @@
       <c r="DC43" s="1"/>
       <c r="DD43" s="1"/>
       <c r="DE43" s="1"/>
-      <c r="DF43" s="1"/>
     </row>
-    <row r="44" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5664,9 +5621,8 @@
       <c r="DC44" s="1"/>
       <c r="DD44" s="1"/>
       <c r="DE44" s="1"/>
-      <c r="DF44" s="1"/>
     </row>
-    <row r="45" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5776,9 +5732,8 @@
       <c r="DC45" s="1"/>
       <c r="DD45" s="1"/>
       <c r="DE45" s="1"/>
-      <c r="DF45" s="1"/>
     </row>
-    <row r="46" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -5888,9 +5843,8 @@
       <c r="DC46" s="1"/>
       <c r="DD46" s="1"/>
       <c r="DE46" s="1"/>
-      <c r="DF46" s="1"/>
     </row>
-    <row r="47" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -6000,9 +5954,8 @@
       <c r="DC47" s="1"/>
       <c r="DD47" s="1"/>
       <c r="DE47" s="1"/>
-      <c r="DF47" s="1"/>
     </row>
-    <row r="48" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -6112,9 +6065,8 @@
       <c r="DC48" s="1"/>
       <c r="DD48" s="1"/>
       <c r="DE48" s="1"/>
-      <c r="DF48" s="1"/>
     </row>
-    <row r="49" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6224,9 +6176,8 @@
       <c r="DC49" s="1"/>
       <c r="DD49" s="1"/>
       <c r="DE49" s="1"/>
-      <c r="DF49" s="1"/>
     </row>
-    <row r="50" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -6336,9 +6287,8 @@
       <c r="DC50" s="1"/>
       <c r="DD50" s="1"/>
       <c r="DE50" s="1"/>
-      <c r="DF50" s="1"/>
     </row>
-    <row r="51" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -6448,9 +6398,8 @@
       <c r="DC51" s="1"/>
       <c r="DD51" s="1"/>
       <c r="DE51" s="1"/>
-      <c r="DF51" s="1"/>
     </row>
-    <row r="52" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -6560,9 +6509,8 @@
       <c r="DC52" s="1"/>
       <c r="DD52" s="1"/>
       <c r="DE52" s="1"/>
-      <c r="DF52" s="1"/>
     </row>
-    <row r="53" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6672,9 +6620,8 @@
       <c r="DC53" s="1"/>
       <c r="DD53" s="1"/>
       <c r="DE53" s="1"/>
-      <c r="DF53" s="1"/>
     </row>
-    <row r="54" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6784,9 +6731,8 @@
       <c r="DC54" s="1"/>
       <c r="DD54" s="1"/>
       <c r="DE54" s="1"/>
-      <c r="DF54" s="1"/>
     </row>
-    <row r="55" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6896,9 +6842,8 @@
       <c r="DC55" s="1"/>
       <c r="DD55" s="1"/>
       <c r="DE55" s="1"/>
-      <c r="DF55" s="1"/>
     </row>
-    <row r="56" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -7008,9 +6953,8 @@
       <c r="DC56" s="1"/>
       <c r="DD56" s="1"/>
       <c r="DE56" s="1"/>
-      <c r="DF56" s="1"/>
     </row>
-    <row r="57" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -7120,9 +7064,8 @@
       <c r="DC57" s="1"/>
       <c r="DD57" s="1"/>
       <c r="DE57" s="1"/>
-      <c r="DF57" s="1"/>
     </row>
-    <row r="58" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -7232,9 +7175,8 @@
       <c r="DC58" s="1"/>
       <c r="DD58" s="1"/>
       <c r="DE58" s="1"/>
-      <c r="DF58" s="1"/>
     </row>
-    <row r="59" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -7344,9 +7286,8 @@
       <c r="DC59" s="1"/>
       <c r="DD59" s="1"/>
       <c r="DE59" s="1"/>
-      <c r="DF59" s="1"/>
     </row>
-    <row r="60" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -7456,9 +7397,8 @@
       <c r="DC60" s="1"/>
       <c r="DD60" s="1"/>
       <c r="DE60" s="1"/>
-      <c r="DF60" s="1"/>
     </row>
-    <row r="61" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -7568,9 +7508,8 @@
       <c r="DC61" s="1"/>
       <c r="DD61" s="1"/>
       <c r="DE61" s="1"/>
-      <c r="DF61" s="1"/>
     </row>
-    <row r="62" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -7680,9 +7619,8 @@
       <c r="DC62" s="1"/>
       <c r="DD62" s="1"/>
       <c r="DE62" s="1"/>
-      <c r="DF62" s="1"/>
     </row>
-    <row r="63" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -7792,9 +7730,8 @@
       <c r="DC63" s="1"/>
       <c r="DD63" s="1"/>
       <c r="DE63" s="1"/>
-      <c r="DF63" s="1"/>
     </row>
-    <row r="64" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -7904,9 +7841,8 @@
       <c r="DC64" s="1"/>
       <c r="DD64" s="1"/>
       <c r="DE64" s="1"/>
-      <c r="DF64" s="1"/>
     </row>
-    <row r="65" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -8016,9 +7952,8 @@
       <c r="DC65" s="1"/>
       <c r="DD65" s="1"/>
       <c r="DE65" s="1"/>
-      <c r="DF65" s="1"/>
     </row>
-    <row r="66" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -8128,9 +8063,8 @@
       <c r="DC66" s="1"/>
       <c r="DD66" s="1"/>
       <c r="DE66" s="1"/>
-      <c r="DF66" s="1"/>
     </row>
-    <row r="67" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -8240,9 +8174,8 @@
       <c r="DC67" s="1"/>
       <c r="DD67" s="1"/>
       <c r="DE67" s="1"/>
-      <c r="DF67" s="1"/>
     </row>
-    <row r="68" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -8352,9 +8285,8 @@
       <c r="DC68" s="1"/>
       <c r="DD68" s="1"/>
       <c r="DE68" s="1"/>
-      <c r="DF68" s="1"/>
     </row>
-    <row r="69" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -8464,9 +8396,8 @@
       <c r="DC69" s="1"/>
       <c r="DD69" s="1"/>
       <c r="DE69" s="1"/>
-      <c r="DF69" s="1"/>
     </row>
-    <row r="70" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -8576,9 +8507,8 @@
       <c r="DC70" s="1"/>
       <c r="DD70" s="1"/>
       <c r="DE70" s="1"/>
-      <c r="DF70" s="1"/>
     </row>
-    <row r="71" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -8688,9 +8618,8 @@
       <c r="DC71" s="1"/>
       <c r="DD71" s="1"/>
       <c r="DE71" s="1"/>
-      <c r="DF71" s="1"/>
     </row>
-    <row r="72" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -8800,9 +8729,8 @@
       <c r="DC72" s="1"/>
       <c r="DD72" s="1"/>
       <c r="DE72" s="1"/>
-      <c r="DF72" s="1"/>
     </row>
-    <row r="73" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -8912,9 +8840,8 @@
       <c r="DC73" s="1"/>
       <c r="DD73" s="1"/>
       <c r="DE73" s="1"/>
-      <c r="DF73" s="1"/>
     </row>
-    <row r="74" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -9024,9 +8951,8 @@
       <c r="DC74" s="1"/>
       <c r="DD74" s="1"/>
       <c r="DE74" s="1"/>
-      <c r="DF74" s="1"/>
     </row>
-    <row r="75" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -9136,9 +9062,8 @@
       <c r="DC75" s="1"/>
       <c r="DD75" s="1"/>
       <c r="DE75" s="1"/>
-      <c r="DF75" s="1"/>
     </row>
-    <row r="76" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -9248,9 +9173,8 @@
       <c r="DC76" s="1"/>
       <c r="DD76" s="1"/>
       <c r="DE76" s="1"/>
-      <c r="DF76" s="1"/>
     </row>
-    <row r="77" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -9360,9 +9284,8 @@
       <c r="DC77" s="1"/>
       <c r="DD77" s="1"/>
       <c r="DE77" s="1"/>
-      <c r="DF77" s="1"/>
     </row>
-    <row r="78" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -9472,9 +9395,8 @@
       <c r="DC78" s="1"/>
       <c r="DD78" s="1"/>
       <c r="DE78" s="1"/>
-      <c r="DF78" s="1"/>
     </row>
-    <row r="79" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -9584,9 +9506,8 @@
       <c r="DC79" s="1"/>
       <c r="DD79" s="1"/>
       <c r="DE79" s="1"/>
-      <c r="DF79" s="1"/>
     </row>
-    <row r="80" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -9696,9 +9617,8 @@
       <c r="DC80" s="1"/>
       <c r="DD80" s="1"/>
       <c r="DE80" s="1"/>
-      <c r="DF80" s="1"/>
     </row>
-    <row r="81" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -9808,9 +9728,8 @@
       <c r="DC81" s="1"/>
       <c r="DD81" s="1"/>
       <c r="DE81" s="1"/>
-      <c r="DF81" s="1"/>
     </row>
-    <row r="82" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -9920,9 +9839,8 @@
       <c r="DC82" s="1"/>
       <c r="DD82" s="1"/>
       <c r="DE82" s="1"/>
-      <c r="DF82" s="1"/>
     </row>
-    <row r="83" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -10032,9 +9950,8 @@
       <c r="DC83" s="1"/>
       <c r="DD83" s="1"/>
       <c r="DE83" s="1"/>
-      <c r="DF83" s="1"/>
     </row>
-    <row r="84" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -10144,9 +10061,8 @@
       <c r="DC84" s="1"/>
       <c r="DD84" s="1"/>
       <c r="DE84" s="1"/>
-      <c r="DF84" s="1"/>
     </row>
-    <row r="85" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -10256,9 +10172,8 @@
       <c r="DC85" s="1"/>
       <c r="DD85" s="1"/>
       <c r="DE85" s="1"/>
-      <c r="DF85" s="1"/>
     </row>
-    <row r="86" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -10368,9 +10283,8 @@
       <c r="DC86" s="1"/>
       <c r="DD86" s="1"/>
       <c r="DE86" s="1"/>
-      <c r="DF86" s="1"/>
     </row>
-    <row r="87" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -10480,9 +10394,8 @@
       <c r="DC87" s="1"/>
       <c r="DD87" s="1"/>
       <c r="DE87" s="1"/>
-      <c r="DF87" s="1"/>
     </row>
-    <row r="88" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -10592,9 +10505,8 @@
       <c r="DC88" s="1"/>
       <c r="DD88" s="1"/>
       <c r="DE88" s="1"/>
-      <c r="DF88" s="1"/>
     </row>
-    <row r="89" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -10704,9 +10616,8 @@
       <c r="DC89" s="1"/>
       <c r="DD89" s="1"/>
       <c r="DE89" s="1"/>
-      <c r="DF89" s="1"/>
     </row>
-    <row r="90" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -10816,9 +10727,8 @@
       <c r="DC90" s="1"/>
       <c r="DD90" s="1"/>
       <c r="DE90" s="1"/>
-      <c r="DF90" s="1"/>
     </row>
-    <row r="91" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -10928,9 +10838,8 @@
       <c r="DC91" s="1"/>
       <c r="DD91" s="1"/>
       <c r="DE91" s="1"/>
-      <c r="DF91" s="1"/>
     </row>
-    <row r="92" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -11040,9 +10949,8 @@
       <c r="DC92" s="1"/>
       <c r="DD92" s="1"/>
       <c r="DE92" s="1"/>
-      <c r="DF92" s="1"/>
     </row>
-    <row r="93" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -11152,9 +11060,8 @@
       <c r="DC93" s="1"/>
       <c r="DD93" s="1"/>
       <c r="DE93" s="1"/>
-      <c r="DF93" s="1"/>
     </row>
-    <row r="94" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -11264,9 +11171,8 @@
       <c r="DC94" s="1"/>
       <c r="DD94" s="1"/>
       <c r="DE94" s="1"/>
-      <c r="DF94" s="1"/>
     </row>
-    <row r="95" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -11376,9 +11282,8 @@
       <c r="DC95" s="1"/>
       <c r="DD95" s="1"/>
       <c r="DE95" s="1"/>
-      <c r="DF95" s="1"/>
     </row>
-    <row r="96" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -11488,9 +11393,8 @@
       <c r="DC96" s="1"/>
       <c r="DD96" s="1"/>
       <c r="DE96" s="1"/>
-      <c r="DF96" s="1"/>
     </row>
-    <row r="97" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -11600,9 +11504,8 @@
       <c r="DC97" s="1"/>
       <c r="DD97" s="1"/>
       <c r="DE97" s="1"/>
-      <c r="DF97" s="1"/>
     </row>
-    <row r="98" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -11712,9 +11615,8 @@
       <c r="DC98" s="1"/>
       <c r="DD98" s="1"/>
       <c r="DE98" s="1"/>
-      <c r="DF98" s="1"/>
     </row>
-    <row r="99" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -11824,9 +11726,8 @@
       <c r="DC99" s="1"/>
       <c r="DD99" s="1"/>
       <c r="DE99" s="1"/>
-      <c r="DF99" s="1"/>
     </row>
-    <row r="100" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -11936,9 +11837,8 @@
       <c r="DC100" s="1"/>
       <c r="DD100" s="1"/>
       <c r="DE100" s="1"/>
-      <c r="DF100" s="1"/>
     </row>
-    <row r="101" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -12048,9 +11948,8 @@
       <c r="DC101" s="1"/>
       <c r="DD101" s="1"/>
       <c r="DE101" s="1"/>
-      <c r="DF101" s="1"/>
     </row>
-    <row r="102" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -12160,9 +12059,8 @@
       <c r="DC102" s="1"/>
       <c r="DD102" s="1"/>
       <c r="DE102" s="1"/>
-      <c r="DF102" s="1"/>
     </row>
-    <row r="103" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -12272,9 +12170,8 @@
       <c r="DC103" s="1"/>
       <c r="DD103" s="1"/>
       <c r="DE103" s="1"/>
-      <c r="DF103" s="1"/>
     </row>
-    <row r="104" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -12384,9 +12281,8 @@
       <c r="DC104" s="1"/>
       <c r="DD104" s="1"/>
       <c r="DE104" s="1"/>
-      <c r="DF104" s="1"/>
     </row>
-    <row r="105" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -12496,9 +12392,8 @@
       <c r="DC105" s="1"/>
       <c r="DD105" s="1"/>
       <c r="DE105" s="1"/>
-      <c r="DF105" s="1"/>
     </row>
-    <row r="106" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -12608,9 +12503,8 @@
       <c r="DC106" s="1"/>
       <c r="DD106" s="1"/>
       <c r="DE106" s="1"/>
-      <c r="DF106" s="1"/>
     </row>
-    <row r="107" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -12720,9 +12614,8 @@
       <c r="DC107" s="1"/>
       <c r="DD107" s="1"/>
       <c r="DE107" s="1"/>
-      <c r="DF107" s="1"/>
     </row>
-    <row r="108" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -12832,9 +12725,8 @@
       <c r="DC108" s="1"/>
       <c r="DD108" s="1"/>
       <c r="DE108" s="1"/>
-      <c r="DF108" s="1"/>
     </row>
-    <row r="109" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -12944,9 +12836,8 @@
       <c r="DC109" s="1"/>
       <c r="DD109" s="1"/>
       <c r="DE109" s="1"/>
-      <c r="DF109" s="1"/>
     </row>
-    <row r="110" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -13056,9 +12947,8 @@
       <c r="DC110" s="1"/>
       <c r="DD110" s="1"/>
       <c r="DE110" s="1"/>
-      <c r="DF110" s="1"/>
     </row>
-    <row r="111" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -13168,9 +13058,8 @@
       <c r="DC111" s="1"/>
       <c r="DD111" s="1"/>
       <c r="DE111" s="1"/>
-      <c r="DF111" s="1"/>
     </row>
-    <row r="112" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -13280,9 +13169,8 @@
       <c r="DC112" s="1"/>
       <c r="DD112" s="1"/>
       <c r="DE112" s="1"/>
-      <c r="DF112" s="1"/>
     </row>
-    <row r="113" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -13392,9 +13280,8 @@
       <c r="DC113" s="1"/>
       <c r="DD113" s="1"/>
       <c r="DE113" s="1"/>
-      <c r="DF113" s="1"/>
     </row>
-    <row r="114" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -13504,9 +13391,8 @@
       <c r="DC114" s="1"/>
       <c r="DD114" s="1"/>
       <c r="DE114" s="1"/>
-      <c r="DF114" s="1"/>
     </row>
-    <row r="115" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -13616,9 +13502,8 @@
       <c r="DC115" s="1"/>
       <c r="DD115" s="1"/>
       <c r="DE115" s="1"/>
-      <c r="DF115" s="1"/>
     </row>
-    <row r="116" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -13728,9 +13613,8 @@
       <c r="DC116" s="1"/>
       <c r="DD116" s="1"/>
       <c r="DE116" s="1"/>
-      <c r="DF116" s="1"/>
     </row>
-    <row r="117" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -13840,9 +13724,8 @@
       <c r="DC117" s="1"/>
       <c r="DD117" s="1"/>
       <c r="DE117" s="1"/>
-      <c r="DF117" s="1"/>
     </row>
-    <row r="118" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -13952,9 +13835,8 @@
       <c r="DC118" s="1"/>
       <c r="DD118" s="1"/>
       <c r="DE118" s="1"/>
-      <c r="DF118" s="1"/>
     </row>
-    <row r="119" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -14064,9 +13946,8 @@
       <c r="DC119" s="1"/>
       <c r="DD119" s="1"/>
       <c r="DE119" s="1"/>
-      <c r="DF119" s="1"/>
     </row>
-    <row r="120" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -14176,9 +14057,8 @@
       <c r="DC120" s="1"/>
       <c r="DD120" s="1"/>
       <c r="DE120" s="1"/>
-      <c r="DF120" s="1"/>
     </row>
-    <row r="121" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -14288,9 +14168,8 @@
       <c r="DC121" s="1"/>
       <c r="DD121" s="1"/>
       <c r="DE121" s="1"/>
-      <c r="DF121" s="1"/>
     </row>
-    <row r="122" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -14400,9 +14279,8 @@
       <c r="DC122" s="1"/>
       <c r="DD122" s="1"/>
       <c r="DE122" s="1"/>
-      <c r="DF122" s="1"/>
     </row>
-    <row r="123" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -14512,9 +14390,8 @@
       <c r="DC123" s="1"/>
       <c r="DD123" s="1"/>
       <c r="DE123" s="1"/>
-      <c r="DF123" s="1"/>
     </row>
-    <row r="124" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -14624,9 +14501,8 @@
       <c r="DC124" s="1"/>
       <c r="DD124" s="1"/>
       <c r="DE124" s="1"/>
-      <c r="DF124" s="1"/>
     </row>
-    <row r="125" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -14736,9 +14612,8 @@
       <c r="DC125" s="1"/>
       <c r="DD125" s="1"/>
       <c r="DE125" s="1"/>
-      <c r="DF125" s="1"/>
     </row>
-    <row r="126" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -14848,9 +14723,8 @@
       <c r="DC126" s="1"/>
       <c r="DD126" s="1"/>
       <c r="DE126" s="1"/>
-      <c r="DF126" s="1"/>
     </row>
-    <row r="127" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -14960,9 +14834,8 @@
       <c r="DC127" s="1"/>
       <c r="DD127" s="1"/>
       <c r="DE127" s="1"/>
-      <c r="DF127" s="1"/>
     </row>
-    <row r="128" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -15072,9 +14945,8 @@
       <c r="DC128" s="1"/>
       <c r="DD128" s="1"/>
       <c r="DE128" s="1"/>
-      <c r="DF128" s="1"/>
     </row>
-    <row r="129" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -15184,9 +15056,8 @@
       <c r="DC129" s="1"/>
       <c r="DD129" s="1"/>
       <c r="DE129" s="1"/>
-      <c r="DF129" s="1"/>
     </row>
-    <row r="130" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -15296,9 +15167,8 @@
       <c r="DC130" s="1"/>
       <c r="DD130" s="1"/>
       <c r="DE130" s="1"/>
-      <c r="DF130" s="1"/>
     </row>
-    <row r="131" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -15408,9 +15278,8 @@
       <c r="DC131" s="1"/>
       <c r="DD131" s="1"/>
       <c r="DE131" s="1"/>
-      <c r="DF131" s="1"/>
     </row>
-    <row r="132" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -15520,9 +15389,8 @@
       <c r="DC132" s="1"/>
       <c r="DD132" s="1"/>
       <c r="DE132" s="1"/>
-      <c r="DF132" s="1"/>
     </row>
-    <row r="133" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -15632,9 +15500,8 @@
       <c r="DC133" s="1"/>
       <c r="DD133" s="1"/>
       <c r="DE133" s="1"/>
-      <c r="DF133" s="1"/>
     </row>
-    <row r="134" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -15744,9 +15611,8 @@
       <c r="DC134" s="1"/>
       <c r="DD134" s="1"/>
       <c r="DE134" s="1"/>
-      <c r="DF134" s="1"/>
     </row>
-    <row r="135" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -15856,9 +15722,8 @@
       <c r="DC135" s="1"/>
       <c r="DD135" s="1"/>
       <c r="DE135" s="1"/>
-      <c r="DF135" s="1"/>
     </row>
-    <row r="136" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -15968,9 +15833,8 @@
       <c r="DC136" s="1"/>
       <c r="DD136" s="1"/>
       <c r="DE136" s="1"/>
-      <c r="DF136" s="1"/>
     </row>
-    <row r="137" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -16080,9 +15944,8 @@
       <c r="DC137" s="1"/>
       <c r="DD137" s="1"/>
       <c r="DE137" s="1"/>
-      <c r="DF137" s="1"/>
     </row>
-    <row r="138" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -16192,9 +16055,8 @@
       <c r="DC138" s="1"/>
       <c r="DD138" s="1"/>
       <c r="DE138" s="1"/>
-      <c r="DF138" s="1"/>
     </row>
-    <row r="139" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -16304,9 +16166,8 @@
       <c r="DC139" s="1"/>
       <c r="DD139" s="1"/>
       <c r="DE139" s="1"/>
-      <c r="DF139" s="1"/>
     </row>
-    <row r="140" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -16416,9 +16277,8 @@
       <c r="DC140" s="1"/>
       <c r="DD140" s="1"/>
       <c r="DE140" s="1"/>
-      <c r="DF140" s="1"/>
     </row>
-    <row r="141" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -16528,9 +16388,8 @@
       <c r="DC141" s="1"/>
       <c r="DD141" s="1"/>
       <c r="DE141" s="1"/>
-      <c r="DF141" s="1"/>
     </row>
-    <row r="142" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -16640,9 +16499,8 @@
       <c r="DC142" s="1"/>
       <c r="DD142" s="1"/>
       <c r="DE142" s="1"/>
-      <c r="DF142" s="1"/>
     </row>
-    <row r="143" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -16752,9 +16610,8 @@
       <c r="DC143" s="1"/>
       <c r="DD143" s="1"/>
       <c r="DE143" s="1"/>
-      <c r="DF143" s="1"/>
     </row>
-    <row r="144" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -16864,9 +16721,8 @@
       <c r="DC144" s="1"/>
       <c r="DD144" s="1"/>
       <c r="DE144" s="1"/>
-      <c r="DF144" s="1"/>
     </row>
-    <row r="145" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -16976,9 +16832,8 @@
       <c r="DC145" s="1"/>
       <c r="DD145" s="1"/>
       <c r="DE145" s="1"/>
-      <c r="DF145" s="1"/>
     </row>
-    <row r="146" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -17088,9 +16943,8 @@
       <c r="DC146" s="1"/>
       <c r="DD146" s="1"/>
       <c r="DE146" s="1"/>
-      <c r="DF146" s="1"/>
     </row>
-    <row r="147" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -17200,9 +17054,8 @@
       <c r="DC147" s="1"/>
       <c r="DD147" s="1"/>
       <c r="DE147" s="1"/>
-      <c r="DF147" s="1"/>
     </row>
-    <row r="148" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -17312,9 +17165,8 @@
       <c r="DC148" s="1"/>
       <c r="DD148" s="1"/>
       <c r="DE148" s="1"/>
-      <c r="DF148" s="1"/>
     </row>
-    <row r="149" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -17424,9 +17276,8 @@
       <c r="DC149" s="1"/>
       <c r="DD149" s="1"/>
       <c r="DE149" s="1"/>
-      <c r="DF149" s="1"/>
     </row>
-    <row r="150" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -17536,9 +17387,8 @@
       <c r="DC150" s="1"/>
       <c r="DD150" s="1"/>
       <c r="DE150" s="1"/>
-      <c r="DF150" s="1"/>
     </row>
-    <row r="151" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -17648,9 +17498,8 @@
       <c r="DC151" s="1"/>
       <c r="DD151" s="1"/>
       <c r="DE151" s="1"/>
-      <c r="DF151" s="1"/>
     </row>
-    <row r="152" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -17760,9 +17609,8 @@
       <c r="DC152" s="1"/>
       <c r="DD152" s="1"/>
       <c r="DE152" s="1"/>
-      <c r="DF152" s="1"/>
     </row>
-    <row r="153" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -17872,9 +17720,8 @@
       <c r="DC153" s="1"/>
       <c r="DD153" s="1"/>
       <c r="DE153" s="1"/>
-      <c r="DF153" s="1"/>
     </row>
-    <row r="154" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -17984,9 +17831,8 @@
       <c r="DC154" s="1"/>
       <c r="DD154" s="1"/>
       <c r="DE154" s="1"/>
-      <c r="DF154" s="1"/>
     </row>
-    <row r="155" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -18096,9 +17942,8 @@
       <c r="DC155" s="1"/>
       <c r="DD155" s="1"/>
       <c r="DE155" s="1"/>
-      <c r="DF155" s="1"/>
     </row>
-    <row r="156" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -18208,9 +18053,8 @@
       <c r="DC156" s="1"/>
       <c r="DD156" s="1"/>
       <c r="DE156" s="1"/>
-      <c r="DF156" s="1"/>
     </row>
-    <row r="157" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -18320,9 +18164,8 @@
       <c r="DC157" s="1"/>
       <c r="DD157" s="1"/>
       <c r="DE157" s="1"/>
-      <c r="DF157" s="1"/>
     </row>
-    <row r="158" spans="1:110" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:109" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -18432,30 +18275,29 @@
       <c r="DC158" s="1"/>
       <c r="DD158" s="1"/>
       <c r="DE158" s="1"/>
-      <c r="DF158" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AO15:AQ15"/>
-    <mergeCell ref="AR16:AT16"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="V10:Z10"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="AD12:AF12"/>
-    <mergeCell ref="AG13:AI13"/>
-    <mergeCell ref="AJ14:AN14"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="BD4:BJ4"/>
-    <mergeCell ref="BK4:BQ4"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="G7:N7"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="T4:Z4"/>
+    <mergeCell ref="AA4:AG4"/>
+    <mergeCell ref="AV4:BB4"/>
+    <mergeCell ref="BC4:BI4"/>
+    <mergeCell ref="BJ4:BP4"/>
+    <mergeCell ref="BQ4:BW4"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="AH4:AN4"/>
+    <mergeCell ref="AO4:AU4"/>
+    <mergeCell ref="AN15:AP15"/>
+    <mergeCell ref="AQ16:AS16"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="U10:Y10"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="AC12:AE12"/>
+    <mergeCell ref="AF13:AH13"/>
+    <mergeCell ref="AI14:AM14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>